<commit_message>
add Log4j2 configuration and ActionHelper Class
</commit_message>
<xml_diff>
--- a/resources/Employees.xlsx
+++ b/resources/Employees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>FIRSTNAME</t>
   </si>
@@ -45,6 +45,42 @@
   </si>
   <si>
     <t>Clarusway</t>
+  </si>
+  <si>
+    <t>Shanae</t>
+  </si>
+  <si>
+    <t>Braun</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Ernser</t>
+  </si>
+  <si>
+    <t>Jamey</t>
+  </si>
+  <si>
+    <t>Weber</t>
+  </si>
+  <si>
+    <t>Jame</t>
+  </si>
+  <si>
+    <t>Senger</t>
+  </si>
+  <si>
+    <t>Angelo</t>
+  </si>
+  <si>
+    <t>Leffler</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>TestLastName</t>
   </si>
 </sst>
 </file>
@@ -89,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -143,6 +179,54 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>